<commit_message>
added Mike's FW Setup to create aoi from shp function. Not finished.
</commit_message>
<xml_diff>
--- a/autoast/test.xlsx
+++ b/autoast/test.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="18">
   <si>
     <t>region</t>
   </si>
@@ -63,20 +63,34 @@
     <t>thompson_okanagan</t>
   </si>
   <si>
-    <t>T:\test</t>
-  </si>
-  <si>
     <t>W:\srm\nel\Local\Geomatics\Workarea\csostad\GitHubAutoAST\gss_authorizations\autoast\aoi.kml</t>
+  </si>
+  <si>
+    <t>\\spatialfiles.bcgov\work\srm\nel\Local\Geomatics\Workarea\csostad\GitHubAutoAST\gss_authorizations\autoast\aoi.shp</t>
+  </si>
+  <si>
+    <t>T:\test1</t>
+  </si>
+  <si>
+    <t>T:\test2</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -99,14 +113,17 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="1" applyNumberFormat="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -407,10 +424,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M2"/>
+  <dimension ref="A1:M8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -473,8 +490,22 @@
         <v>15</v>
       </c>
       <c r="F2" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>13</v>
+      </c>
+      <c r="B3" t="s">
         <v>14</v>
       </c>
+      <c r="F3" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="B8" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>